<commit_message>
Added a shift ## to
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -88,10 +88,10 @@
     <t>Ссылка на поручение</t>
   </si>
   <si>
-    <t>Входящий документ##Письмо</t>
-  </si>
-  <si>
-    <t>0551-01993-25##01.07.2025</t>
+    <t>Входящий документ Письмо</t>
+  </si>
+  <si>
+    <t>0551-01993-25 01.07.2025</t>
   </si>
   <si>
     <t>Касательно проведения анализа  деятельности имеющихся обособленных подразделений и их реквизитов</t>
@@ -109,7 +109,7 @@
     <t>Общество с ограниченной ответственностью "Сибирская Интернет Компания"</t>
   </si>
   <si>
-    <t>ИП-00038-АИ-25##01.07.2025</t>
+    <t>ИП-00038-АИ-25 01.07.2025</t>
   </si>
   <si>
     <t>Исполнить документ</t>
@@ -139,7 +139,7 @@
     <t>Закрыто</t>
   </si>
   <si>
-    <t>Поручение вне компетенции. Деятельность обособленных подразделений в зоне компетенции юридической службы Общества.##02.07.2025</t>
+    <t>Поручение вне компетенции. Деятельность обособленных подразделений в зоне компетенции юридической службы Общества. 02.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/4379edc1-3b58-45dc-8bfb-9e66dd2324e8</t>
@@ -148,7 +148,7 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/e43439bd-2dd2-44e8-88c8-398abae1433e</t>
   </si>
   <si>
-    <t>0551-01958-25##01.07.2025</t>
+    <t>0551-01958-25 01.07.2025</t>
   </si>
   <si>
     <t>О вовлечении в производство имеющихся запасов</t>
@@ -157,7 +157,7 @@
     <t>Исполнен</t>
   </si>
   <si>
-    <t>ИП-00045-АИ-25##02.07.2025</t>
+    <t>ИП-00045-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Слепченко М.Н.</t>
@@ -169,7 +169,7 @@
     <t>16.07.2025</t>
   </si>
   <si>
-    <t>Ответ направлен в рабочем порядке (вложение).##09.07.2025</t>
+    <t>Ответ направлен в рабочем порядке (вложение). 09.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/3bf6f9f5-aed7-4ffd-902f-bd0860f4fe51</t>
@@ -178,16 +178,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/eaf5a994-9751-48e6-9b6f-f34ca810cc54</t>
   </si>
   <si>
-    <t>Входящий документ##Претензия</t>
-  </si>
-  <si>
-    <t>0551-01999-25##01.07.2025</t>
+    <t>Входящий документ Претензия</t>
+  </si>
+  <si>
+    <t>0551-01999-25 01.07.2025</t>
   </si>
   <si>
     <t>О нарушении обязательств по договору от 29.12.2021 №2322021/1777Д/1В1121/15008Д</t>
   </si>
   <si>
-    <t>ИП-00032-АИ-25##01.07.2025</t>
+    <t>ИП-00032-АИ-25 01.07.2025</t>
   </si>
   <si>
     <t>Кленин С.Е.</t>
@@ -205,7 +205,7 @@
     <t>11.07.2025</t>
   </si>
   <si>
-    <t>Претензия обоснованная. Согласование ЮС получено. Направлен ответ №ИСХ-МВ-00838-25 от 10.07.2025 г.##11.07.2025</t>
+    <t>Претензия обоснованная. Согласование ЮС получено. Направлен ответ №ИСХ-МВ-00838-25 от 10.07.2025 г. 11.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/494f3a73-0a97-426c-a212-fbc421c6c8a1</t>
@@ -214,13 +214,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/e65b3f46-ab30-41d7-b7bd-b3a6ea3604eb</t>
   </si>
   <si>
-    <t>0551-02001-25##01.07.2025</t>
+    <t>0551-02001-25 01.07.2025</t>
   </si>
   <si>
     <t>Предложение рассмотреть возможность приобретения конструкций для физической антидроновой защиты инфраструктурных объектов в рамках современных реалий: конструкций для физической защиты инфраструктурных объектов, многогранных и решетчатых опор ЛЭП 6-500кВ, опор освещения и контактных сетей, мачт сотовой связи, - металлоконструкций общестроительного и специального назначения; провести рабочую встречу (ООО Научно-производственное объединение «МуромЭнергоМаш» (ООО НПО «МЭМ», г. Муром, Владимирская обл.)</t>
   </si>
   <si>
-    <t>ИП-00039-АИ-25##01.07.2025</t>
+    <t>ИП-00039-АИ-25 01.07.2025</t>
   </si>
   <si>
     <t>Филатова Ю.Н.</t>
@@ -232,7 +232,7 @@
     <t>04.07.2025</t>
   </si>
   <si>
-    <t>Физическая защита не является профильной деятельностью для ИТ интегратора. ##04.07.2025</t>
+    <t>Физическая защита не является профильной деятельностью для ИТ интегратора.  04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/1b1459f9-fed2-4160-ac78-cf15ba54d6cb</t>
@@ -241,16 +241,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/8eea6054-6626-4951-be35-71419f132989</t>
   </si>
   <si>
-    <t>Входящий документ##</t>
-  </si>
-  <si>
-    <t>0551-02062-25##02.07.2025</t>
+    <t xml:space="preserve">Входящий документ </t>
+  </si>
+  <si>
+    <t>0551-02062-25 02.07.2025</t>
   </si>
   <si>
     <t>О направлении протокола совещания от 25.06.2025</t>
   </si>
   <si>
-    <t>ИП-00048-АИ-25##02.07.2025</t>
+    <t>ИП-00048-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Сафин Р.Р.</t>
@@ -262,7 +262,7 @@
     <t>18.07.2025</t>
   </si>
   <si>
-    <t>Информация внесена в протокол ВКС ПБОТОС №25 от 04.07.2025.Отчетность ОГ и ДЗО подготовлена и выложена в ВКД.##18.07.2025</t>
+    <t>Информация внесена в протокол ВКС ПБОТОС №25 от 04.07.2025.Отчетность ОГ и ДЗО подготовлена и выложена в ВКД. 18.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/73a48f86-02a7-4ab5-a68f-2a18471d14a1</t>
@@ -271,13 +271,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/b140fa74-a509-4777-8cf6-5fec8ffb8c56</t>
   </si>
   <si>
-    <t>0551-01994-25##01.07.2025</t>
+    <t>0551-01994-25 01.07.2025</t>
   </si>
   <si>
     <t>О зачете авансового платежа</t>
   </si>
   <si>
-    <t>ИП-00050-АИ-25##02.07.2025</t>
+    <t>ИП-00050-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Раченков В.В.</t>
@@ -286,7 +286,7 @@
     <t>05.08.2025</t>
   </si>
   <si>
-    <t>Письмо 245 от 25.06.2025 поступило ранее в    ООО "РН-Учет", отражено в учетной системе при закрытии июня 2025 г.##01.08.2025</t>
+    <t>Письмо 245 от 25.06.2025 поступило ранее в    ООО "РН-Учет", отражено в учетной системе при закрытии июня 2025 г. 01.08.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/406387be-5a9e-4cc0-91e9-7a293c79a851</t>
@@ -295,13 +295,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/81381b9a-4ddc-49b9-8694-9f1fd07a67e8</t>
   </si>
   <si>
-    <t>0551-02076-25##02.07.2025</t>
+    <t>0551-02076-25 02.07.2025</t>
   </si>
   <si>
     <t>Благодарность проектной команде ИТ-проектаIID-1338 в части модификации функциональности и подключения ОГ 2-ой очереди к ИПР ФБ ОЭЭЭС</t>
   </si>
   <si>
-    <t>ИП-00065-АИ-25##02.07.2025</t>
+    <t>ИП-00065-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Барсуков А.Г.</t>
@@ -313,7 +313,7 @@
     <t>08.07.2025</t>
   </si>
   <si>
-    <t>Использован финальный отчет &lt;a href='#' onclick="LogicECM.module.Base.Util.viewAttributes({itemId:'workspace://SpacesStore/d22c6db8-b653-44ea-92ed-c698d2505fcd'}); return false;"&gt;Калинина Н.А.&lt;/a&gt; из &lt;a href='#' onclick="LogicECM.module.Base.Util.viewAttributes({itemId:'workspace://SpacesStore/107a230b-f53e-419f-a0f5-042845fdedce'}); return false;"&gt;К поручению ИП-00065-АИ-25&lt;/a&gt; : Сотрудники СИБИНТЕК в списках отсутствуют.Для организации премирования из ФГД работников СИБИНТЕК -СОФТ письмо и дополненный список работников направлены Егоровой Л.А.##08.07.2025</t>
+    <t>Использован финальный отчет &lt;a href='#' onclick="LogicECM.module.Base.Util.viewAttributes({itemId:'workspace://SpacesStore/d22c6db8-b653-44ea-92ed-c698d2505fcd'}); return false;"&gt;Калинина Н.А.&lt;/a&gt; из &lt;a href='#' onclick="LogicECM.module.Base.Util.viewAttributes({itemId:'workspace://SpacesStore/107a230b-f53e-419f-a0f5-042845fdedce'}); return false;"&gt;К поручению ИП-00065-АИ-25&lt;/a&gt; : Сотрудники СИБИНТЕК в списках отсутствуют.Для организации премирования из ФГД работников СИБИНТЕК -СОФТ письмо и дополненный список работников направлены Егоровой Л.А. 08.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/0d87ee56-5c7b-417c-852c-a0016576db9c</t>
@@ -322,16 +322,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/6237b1d4-894d-435f-aba6-d40d386bedb0</t>
   </si>
   <si>
-    <t>0551-02089-25##02.07.2025</t>
+    <t>0551-02089-25 02.07.2025</t>
   </si>
   <si>
     <t>О возможности вовлечения МТР</t>
   </si>
   <si>
-    <t>ИП-00066-АИ-25##02.07.2025</t>
-  </si>
-  <si>
-    <t>Ответ направлен в рабочем порядке (вложение).##11.07.2025</t>
+    <t>ИП-00066-АИ-25 02.07.2025</t>
+  </si>
+  <si>
+    <t>Ответ направлен в рабочем порядке (вложение). 11.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/9f3b27ad-873c-485d-94fd-e21cfb5afd8e</t>
@@ -340,13 +340,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/2b32d298-715a-4a6a-8a2f-0cbcd57ccd7f</t>
   </si>
   <si>
-    <t>0551-02095-25##02.07.2025</t>
+    <t>0551-02095-25 02.07.2025</t>
   </si>
   <si>
     <t>О приглашении на встречу с психологом 03.07.2025</t>
   </si>
   <si>
-    <t>ИП-00067-АИ-25##02.07.2025</t>
+    <t>ИП-00067-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Низамов Р.Р.</t>
@@ -358,7 +358,7 @@
     <t>03.07.2025</t>
   </si>
   <si>
-    <t>Принято в работу. Доведено до заинтересованных лиц.##03.07.2025</t>
+    <t>Принято в работу. Доведено до заинтересованных лиц. 03.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/6e81c7dc-6ec9-43ac-9c2e-283697503a76</t>
@@ -367,19 +367,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/4ba5034b-5877-4183-acb3-21815e83ea06</t>
   </si>
   <si>
-    <t>0551-02052-25##02.07.2025</t>
+    <t>0551-02052-25 02.07.2025</t>
   </si>
   <si>
     <t>О предоставлении информации</t>
   </si>
   <si>
-    <t>ИП-00068-АИ-25##02.07.2025</t>
+    <t>ИП-00068-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>15.07.2025</t>
   </si>
   <si>
-    <t>Направлен ответ (№ ИСХ-ЦА-01263-25 от 15.07.2025.) ##16.07.2025</t>
+    <t>Направлен ответ (№ ИСХ-ЦА-01263-25 от 15.07.2025.)  16.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/4048d7db-5164-4519-81de-55aa02fb437a</t>
@@ -388,13 +388,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/83065ec2-97d8-4962-9825-b2b9e72aaef3</t>
   </si>
   <si>
-    <t>0551-02050-25##02.07.2025</t>
+    <t>0551-02050-25 02.07.2025</t>
   </si>
   <si>
     <t>Уведомление № 99-253-02468 о необходимости внесения разовой платы и ежегодной платы за первый период использования радиочастотного спектра</t>
   </si>
   <si>
-    <t>ИП-00069-АИ-25##02.07.2025</t>
+    <t>ИП-00069-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Егоркина Е.В.</t>
@@ -409,7 +409,7 @@
     <t>03.08.2025</t>
   </si>
   <si>
-    <t>По уведомлению №99-253-02468 разовая и ежегодная плата внесена##28.07.2025</t>
+    <t>По уведомлению №99-253-02468 разовая и ежегодная плата внесена 28.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/e5af315d-4c59-4b53-92ce-f04ef0f13a53</t>
@@ -418,19 +418,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/17d00fc8-e7c5-4d74-872c-c70e5d9377bc</t>
   </si>
   <si>
-    <t>0551-02043-25##02.07.2025</t>
+    <t>0551-02043-25 02.07.2025</t>
   </si>
   <si>
     <t>О направлении информации</t>
   </si>
   <si>
-    <t>ИП-00071-АИ-25##02.07.2025</t>
+    <t>ИП-00071-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>10.07.2025</t>
   </si>
   <si>
-    <t>В Конкурсе принимать участие не будем, т.к. профессии, по которым проводится Конкурс - не нашего профиля.##03.07.2025</t>
+    <t>В Конкурсе принимать участие не будем, т.к. профессии, по которым проводится Конкурс - не нашего профиля. 03.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/310cb83e-9c42-4640-a8fa-1e6b85dd7ff0</t>
@@ -439,19 +439,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/075e7d85-01dc-4487-b394-2e9602efcc89</t>
   </si>
   <si>
-    <t>0551-02045-25##02.07.2025</t>
+    <t>0551-02045-25 02.07.2025</t>
   </si>
   <si>
     <t>О согласовании оснащения лизинговых ТС системами мониторинга водителей (СМВ)</t>
   </si>
   <si>
-    <t>ИП-00074-АИ-25##02.07.2025</t>
+    <t>ИП-00074-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Фурсов В.В.</t>
   </si>
   <si>
-    <t>Принято для использования в работе.Доведено до УСиЛ МР.В настоящее время по функции отсутствуют арендованные ТС ООО "Нефтепромлизинг".##09.07.2025</t>
+    <t>Принято для использования в работе.Доведено до УСиЛ МР.В настоящее время по функции отсутствуют арендованные ТС ООО "Нефтепромлизинг". 09.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/37d26527-6268-46c6-9e5c-ec38b7e054ab</t>
@@ -460,16 +460,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/c06e65f3-405b-4792-bf01-ff35a4e4dcfc</t>
   </si>
   <si>
-    <t>0551-02066-25##02.07.2025</t>
+    <t>0551-02066-25 02.07.2025</t>
   </si>
   <si>
     <t>О проведении заседаний Комиссии по контролю ПАО «НК «Роснефть» в 2025 г.</t>
   </si>
   <si>
-    <t>ИП-00075-АИ-25##02.07.2025</t>
-  </si>
-  <si>
-    <t>В План-графике проведения заседаний на 2025 г. ООО ИК "СИБИНТЕК" не запланировано. Из предыдущих ПКМ по Обществу (МКР Поволжье, декабрь 2023) до настоящего времени не выполнено одно мероприятие - формирование ОС ПБОТОС Общества в соответствии с требованиями ТОС Компании. Данное поручение на контроле и исполнении, ОС согласована в Компании, внедрение запланировано до конца 2025 года.ответа не требует##08.07.2025</t>
+    <t>ИП-00075-АИ-25 02.07.2025</t>
+  </si>
+  <si>
+    <t>В План-графике проведения заседаний на 2025 г. ООО ИК "СИБИНТЕК" не запланировано. Из предыдущих ПКМ по Обществу (МКР Поволжье, декабрь 2023) до настоящего времени не выполнено одно мероприятие - формирование ОС ПБОТОС Общества в соответствии с требованиями ТОС Компании. Данное поручение на контроле и исполнении, ОС согласована в Компании, внедрение запланировано до конца 2025 года.ответа не требует 08.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/f37468ea-c3a2-498e-983d-1bbe484a05b0</t>
@@ -478,13 +478,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/b8884267-ac64-44ac-a105-7277eaa6fdba</t>
   </si>
   <si>
-    <t>0551-02060-25##02.07.2025</t>
+    <t>0551-02060-25 02.07.2025</t>
   </si>
   <si>
     <t>Об анализе реагирования на чрезвычайные ситуации (происшествия) в июне 2025 года</t>
   </si>
   <si>
-    <t>ИП-00076-АИ-25##02.07.2025</t>
+    <t>ИП-00076-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>07.07.2025</t>
@@ -493,7 +493,7 @@
     <t>14.07.2025</t>
   </si>
   <si>
-    <t>Исполнено. Доведено по функции до филиалов и ДЗО на совещании руководителей и специалистов службы ПБОТОС и ГОЧС ООО ИК «СИБИНТЕК», протокол ВКС № 25 от 04.07.25ответа не требует##07.07.2025</t>
+    <t>Исполнено. Доведено по функции до филиалов и ДЗО на совещании руководителей и специалистов службы ПБОТОС и ГОЧС ООО ИК «СИБИНТЕК», протокол ВКС № 25 от 04.07.25ответа не требует 07.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/e3b707df-211c-455b-82e8-fbbb02dbcf6b</t>
@@ -502,16 +502,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/20ce005a-a9b7-4a6b-8f1a-93aad0b066d8</t>
   </si>
   <si>
-    <t>0551-01936-25##01.07.2025</t>
+    <t>0551-01936-25 01.07.2025</t>
   </si>
   <si>
     <t>О направлении информационного листка</t>
   </si>
   <si>
-    <t>ИП-00078-АИ-25##02.07.2025</t>
-  </si>
-  <si>
-    <t>Исполнено. Доведено по функции до филиалов и ДЗО на совещании руководителей и специалистов службы ПБОТОС и ГОЧС ООО ИК «СИБИНТЕК», протокол ВКС № 25 от 04.07.25данный вид работ для общества не свойственен, не эксплуатируются данные виды ТС ответа не требуется##08.07.2025</t>
+    <t>ИП-00078-АИ-25 02.07.2025</t>
+  </si>
+  <si>
+    <t>Исполнено. Доведено по функции до филиалов и ДЗО на совещании руководителей и специалистов службы ПБОТОС и ГОЧС ООО ИК «СИБИНТЕК», протокол ВКС № 25 от 04.07.25данный вид работ для общества не свойственен, не эксплуатируются данные виды ТС ответа не требуется 08.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/d48322b8-6a3c-4906-9a2c-bc38775b9a41</t>
@@ -520,7 +520,7 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/0e5e45af-b6a2-4a5c-bd3c-406bce20ed95</t>
   </si>
   <si>
-    <t>ИП-00086-АИ-25##02.07.2025</t>
+    <t>ИП-00086-АИ-25 02.07.2025</t>
   </si>
   <si>
     <t>Шилов А.В.</t>
@@ -535,16 +535,16 @@
     <t>09.07.2025 18:00</t>
   </si>
   <si>
-    <t>Консолидированная информация по ОП Общества подготовлена в формате xlsписьмо в РН-Учет подготовлено, направлено на согласование и подписание ГД##08.07.2025</t>
+    <t>Консолидированная информация по ОП Общества подготовлена в формате xlsписьмо в РН-Учет подготовлено, направлено на согласование и подписание ГД 08.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/78d0f2f2-07ea-4ea7-8264-cfac675bc9ad</t>
   </si>
   <si>
-    <t>Поручение##</t>
-  </si>
-  <si>
-    <t>П-13494-95-25 - п.1##02.07.2025</t>
+    <t xml:space="preserve">Поручение </t>
+  </si>
+  <si>
+    <t>П-13494-95-25 - п.1 02.07.2025</t>
   </si>
   <si>
     <t>Организовать работу</t>
@@ -553,7 +553,7 @@
     <t>На внешнем контроле</t>
   </si>
   <si>
-    <t>К поручению П-13494-95-25 - п.1##02.07.2025</t>
+    <t>К поручению П-13494-95-25 - п.1 02.07.2025</t>
   </si>
   <si>
     <t>Мерцалов И.В.</t>
@@ -568,7 +568,7 @@
     <t>22.07.2025</t>
   </si>
   <si>
-    <t>По информации от Д.А. Мискетова.От ответственных ДИиРБП в ОГ направлено письмо от 13.05.2025 (вложение 2) для получения разъяснений о причинах нарушения требований закупочных процедур.Поэтому на текущий момент предоставление позиции по поручению П-13494-95-25-п.1 от 03.07.2025 от Сибинтек и С-Софт не требуется (вложение).Позиция от С-Софт на П-09783-95-25 - п.1 (И-2025-06163 от 07.05.2025, вложение 1) направлена Д.А. Мискетову.##22.07.2025</t>
+    <t>По информации от Д.А. Мискетова.От ответственных ДИиРБП в ОГ направлено письмо от 13.05.2025 (вложение 2) для получения разъяснений о причинах нарушения требований закупочных процедур.Поэтому на текущий момент предоставление позиции по поручению П-13494-95-25-п.1 от 03.07.2025 от Сибинтек и С-Софт не требуется (вложение).Позиция от С-Софт на П-09783-95-25 - п.1 (И-2025-06163 от 07.05.2025, вложение 1) направлена Д.А. Мискетову. 22.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/e93978f6-d44c-4282-8bff-c6fc70188ede</t>
@@ -577,16 +577,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/bc41fc5f-6187-46d7-9730-c984d5209a90</t>
   </si>
   <si>
-    <t>0551-02056-25##02.07.2025</t>
+    <t>0551-02056-25 02.07.2025</t>
   </si>
   <si>
     <t>О формировании перечня технических характеристик БПЛА</t>
   </si>
   <si>
-    <t>ИП-00091-АИ-25##02.07.2025</t>
-  </si>
-  <si>
-    <t>На текущий момент нет текущих и планируемых активностей по использованию БПЛА.При этом Сибинтек участвует в  Программе Компании по обнаружению и устранению утечек углеводородов (вкл. метан), а также оказывает экспертную технологическую и методологическую поддержку ЦАУК (Департамент развития международных проектов и энергетической трансформации) по управлению мероприятиями по воздушным обследованиям с помощью беспилотных воздушных судов в ОГ в рамках консалтингового договора с ПАО «НК «Роснефть». Сами воздушные обследования выполняются внешними контрагентами.##11.07.2025</t>
+    <t>ИП-00091-АИ-25 02.07.2025</t>
+  </si>
+  <si>
+    <t>На текущий момент нет текущих и планируемых активностей по использованию БПЛА.При этом Сибинтек участвует в  Программе Компании по обнаружению и устранению утечек углеводородов (вкл. метан), а также оказывает экспертную технологическую и методологическую поддержку ЦАУК (Департамент развития международных проектов и энергетической трансформации) по управлению мероприятиями по воздушным обследованиям с помощью беспилотных воздушных судов в ОГ в рамках консалтингового договора с ПАО «НК «Роснефть». Сами воздушные обследования выполняются внешними контрагентами. 11.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/2f467d0c-1ace-46d4-96c3-946213da5049</t>
@@ -595,13 +595,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/381ccd2d-d969-4727-9572-01eaa7c2ea14</t>
   </si>
   <si>
-    <t>0551-01997-25##01.07.2025</t>
+    <t>0551-01997-25 01.07.2025</t>
   </si>
   <si>
     <t>О наделении полномочиями сотрудника</t>
   </si>
   <si>
-    <t>ИП-00121-АИ-25##03.07.2025</t>
+    <t>ИП-00121-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>02.08.2025</t>
@@ -613,7 +613,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>Информация принята.Инструкция по доступам направлена ответственному от РН-Сервис.##04.08.2025</t>
+    <t>Информация принята.Инструкция по доступам направлена ответственному от РН-Сервис. 04.08.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/dbd20c46-f9a3-43a8-8e5c-d0404517322e</t>
@@ -622,19 +622,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/1b38ffa8-444e-4b36-b7dc-6a09420821e9</t>
   </si>
   <si>
-    <t>0551-02236-25##03.07.2025</t>
+    <t>0551-02236-25 03.07.2025</t>
   </si>
   <si>
     <t>Об участии в Международном форуме по развитию беспилотных систем, 7-17 августа 2025 г., в Москве (Пр-589 от 19.03.2025) (  АНО «Платформа НТИ»)</t>
   </si>
   <si>
-    <t>ИП-00130-АИ-25##03.07.2025</t>
+    <t>ИП-00130-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>25.07.2025 18:00</t>
   </si>
   <si>
-    <t>Участие не планируется##09.07.2025</t>
+    <t>Участие не планируется 09.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/d2a79c91-d988-4f2c-8559-648999246710</t>
@@ -643,16 +643,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/a6e41f48-9620-4b58-92ca-60f2aaeed392</t>
   </si>
   <si>
-    <t>0551-02115-25##02.07.2025</t>
+    <t>0551-02115-25 02.07.2025</t>
   </si>
   <si>
     <t>Об организации строительного контроля</t>
   </si>
   <si>
-    <t>ИП-00138-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>График сменности специалистов РН-Стройконтроль учтен в работе и доведен до ответственных лиц как в ЦА, так и в филиале "МР Западная Сибирь". Ответ не требуется, письмо тинформационное.##03.07.2025</t>
+    <t>ИП-00138-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>График сменности специалистов РН-Стройконтроль учтен в работе и доведен до ответственных лиц как в ЦА, так и в филиале "МР Западная Сибирь". Ответ не требуется, письмо тинформационное. 03.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/c67598a7-957e-489e-98a5-bee595c4f71a</t>
@@ -661,13 +661,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/850851db-1e78-46b4-b0ad-d0906c869fab</t>
   </si>
   <si>
-    <t>0551-01935-25##01.07.2025</t>
+    <t>0551-01935-25 01.07.2025</t>
   </si>
   <si>
     <t>Претензионное письмо по объектам ЛСО дог. №625/20 филиал «Макрорегион Урал» ООО ИК «СИБИНТЕК»</t>
   </si>
   <si>
-    <t>ИП-00139-АИ-25##03.07.2025</t>
+    <t>ИП-00139-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>Симонов А.Ю.</t>
@@ -682,7 +682,7 @@
     <t>25.07.2025</t>
   </si>
   <si>
-    <t>Ответ направлен ##25.07.2025</t>
+    <t>Ответ направлен  25.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/d1bc4844-5d6f-40ae-ba75-d4a67e312850</t>
@@ -691,13 +691,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/583e573d-cb0b-464b-86be-36ae98b75f3a</t>
   </si>
   <si>
-    <t>0551-02112-25##02.07.2025</t>
+    <t>0551-02112-25 02.07.2025</t>
   </si>
   <si>
     <t>О приглашении к участию в корпоративных соревнованиях по шахматам и настольному теннису 13-14 сентября 2025 г. в Москве</t>
   </si>
   <si>
-    <t>ИП-00140-АИ-25##03.07.2025</t>
+    <t>ИП-00140-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>Лудина М.А.</t>
@@ -712,7 +712,7 @@
     <t>14</t>
   </si>
   <si>
-    <t>##</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/0c2f733c-664b-444d-8cdb-a7e94dec0125</t>
@@ -721,16 +721,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/7161beb5-b19a-48bd-81d1-b80344cc438b</t>
   </si>
   <si>
-    <t>0551-02136-25##02.07.2025</t>
+    <t>0551-02136-25 02.07.2025</t>
   </si>
   <si>
     <t>Об обеспечении смазочными материалами и присадками дочерних и зависимых обществ ПАО "НК "Роснефть"</t>
   </si>
   <si>
-    <t>ИП-00141-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Принято для работы. Доведено до УСиЛ МР для использования в работе.##09.07.2025</t>
+    <t>ИП-00141-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Принято для работы. Доведено до УСиЛ МР для использования в работе. 09.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/65b7bad6-dce4-48cc-98ee-7666de49d558</t>
@@ -739,19 +739,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/dfa6c8cf-ca5e-42d6-bef7-dfc670a240e1</t>
   </si>
   <si>
-    <t>0551-02235-25##03.07.2025</t>
+    <t>0551-02235-25 03.07.2025</t>
   </si>
   <si>
     <t>Извещение о принесении кассационной жалобы Бойчук А.Н.</t>
   </si>
   <si>
-    <t>ИП-00143-АИ-25##03.07.2025</t>
+    <t>ИП-00143-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>20.08.2025</t>
   </si>
   <si>
-    <t>Передано в работу судебному представителю.##04.07.2025</t>
+    <t>Передано в работу судебному представителю. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/90388942-969a-4c11-a7bb-0c74c8cbc3fb</t>
@@ -760,16 +760,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/509bb8ff-bf14-4180-aa33-f860c38e8d66</t>
   </si>
   <si>
-    <t>0551-02193-25##03.07.2025</t>
+    <t>0551-02193-25 03.07.2025</t>
   </si>
   <si>
     <t>О приглашении к участию в производственном совещании ООО «РН-Учет» 11.07.2025</t>
   </si>
   <si>
-    <t>ИП-00150-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>присутствовал на встрече ##15.07.2025</t>
+    <t>ИП-00150-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>присутствовал на встрече  15.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/a1409c09-3bdc-4eec-8329-53ec3c349a2f</t>
@@ -778,16 +778,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/76f6ea85-5aed-4a74-b2b5-30d81695be8a</t>
   </si>
   <si>
-    <t>0551-02187-25##03.07.2025</t>
+    <t>0551-02187-25 03.07.2025</t>
   </si>
   <si>
     <t>О согласовании участия в закрытых процедурах закупок оборудования CISCO, FLUKE</t>
   </si>
   <si>
-    <t>ИП-00151-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Принято для информации.Потенциальный КА включен в лист ожидания.##04.07.2025</t>
+    <t>ИП-00151-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Принято для информации.Потенциальный КА включен в лист ожидания. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/00a2bda9-329d-40a1-a24a-92428152c910</t>
@@ -796,13 +796,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/957a590a-92d3-4786-8988-0e19ebb41661</t>
   </si>
   <si>
-    <t>0551-02254-25##03.07.2025</t>
+    <t>0551-02254-25 03.07.2025</t>
   </si>
   <si>
     <t>Об анализе информирования и представления донесений при возникновении ЧС (происшествий) во II квартале 2025 года</t>
   </si>
   <si>
-    <t>ИП-00153-АИ-25##03.07.2025</t>
+    <t>ИП-00153-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/29d4b0df-648a-4d11-a452-4023596ec405</t>
@@ -811,16 +811,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/b8daffa7-d744-4e31-b754-8c465ee1240f</t>
   </si>
   <si>
-    <t>0551-02300-25##03.07.2025</t>
+    <t>0551-02300-25 03.07.2025</t>
   </si>
   <si>
     <t>Об исполнении мероприятий месячника безопасности</t>
   </si>
   <si>
-    <t>ИП-00154-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>В адрес куратора договора в рабочем порядке направлены листы ознакомления (конверт) ##22.07.2025</t>
+    <t>ИП-00154-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>В адрес куратора договора в рабочем порядке направлены листы ознакомления (конверт)  22.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/c3c59dfb-270c-492a-8950-83a81d2bd170</t>
@@ -829,16 +829,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/893e4293-ba48-4a67-aba5-3c0781302c5c</t>
   </si>
   <si>
-    <t>0551-02183-25##03.07.2025</t>
+    <t>0551-02183-25 03.07.2025</t>
   </si>
   <si>
     <t>Об организации командировки работника в ООО "РН-Юганскнефтегаз"</t>
   </si>
   <si>
-    <t>ИП-00156-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Отчет Соисполнителя подчиненного поручения Шокурова Е.А., направлен 08.07.2025:  ДС в БП предусмотрены, готовится проект ответа в Службу Снабжения.##10.07.2025</t>
+    <t>ИП-00156-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Отчет Соисполнителя подчиненного поручения Шокурова Е.А., направлен 08.07.2025:  ДС в БП предусмотрены, готовится проект ответа в Службу Снабжения. 10.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/912a8ef9-1dad-4109-a0cf-c048c00b31cd</t>
@@ -847,13 +847,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/a6b730c7-0926-464e-bf57-3e8fe7485ffe</t>
   </si>
   <si>
-    <t>0551-02267-25##03.07.2025</t>
+    <t>0551-02267-25 03.07.2025</t>
   </si>
   <si>
     <t>Об успешном выполнении работ и завершенииИТ-проекта IID-1220</t>
   </si>
   <si>
-    <t>ИП-00157-АИ-25##03.07.2025</t>
+    <t>ИП-00157-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>Мокрецов А.В.</t>
@@ -868,16 +868,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/80977d60-0971-4b96-8508-f2cffcfb43f2</t>
   </si>
   <si>
-    <t>0551-02290-25##03.07.2025</t>
+    <t>0551-02290-25 03.07.2025</t>
   </si>
   <si>
     <t>Апелляционная жалоба (краткая) по гражданском делу № 02-0718/2025</t>
   </si>
   <si>
-    <t>ИП-00158-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Передано в работу судебному представителю##04.07.2025</t>
+    <t>ИП-00158-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Передано в работу судебному представителю 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/cf6f9fc3-3e33-422b-9f75-a76a75f9f56f</t>
@@ -886,13 +886,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/b93d6bd6-9813-4c54-b711-91006c0fdb7f</t>
   </si>
   <si>
-    <t>0551-02313-25##03.07.2025</t>
+    <t>0551-02313-25 03.07.2025</t>
   </si>
   <si>
     <t>О направлении материалов ВКС</t>
   </si>
   <si>
-    <t>ИП-00159-АИ-25##03.07.2025</t>
+    <t>ИП-00159-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>30.07.2025</t>
@@ -901,7 +901,7 @@
     <t>17.07.2025</t>
   </si>
   <si>
-    <t>п. 2 – проведено совещание с работниками Блока ПБОТОС и ГОЧС (Протокол ВКС от 11.07.2025 №26). В целях уточнения п. 9.7.1 Методических указаний Компании «Взаимодействие с подрядными организациями в области промышленной и пожарной безопасности, охраны труда и окружающей среды» № П3-05 Р-0881 разработан шаблон варианта «Порядка передачи оперативной информации о возникновении (угрозе возникновения) ЧС природного и техногенного характера, происшествия в филиал при оказании услуг и выполнении работ в интересах ООО ИК «СИБИНТЕК»». В филиалах организовано уточнение разработанного шаблона с учетом рода деятельности/вида оказываемых услуг и направление информационных писем в подрядные организации с уточненным порядком передачи оперативной информации при возникновении (угрозе возникновения) ЧС природного и техногенного характера, происшествия во время оказания услуги и/или выполнения работы по договорам с ООО ИК «СИБИНТЕК» на объектах Компании или Общества.п.8 – учебные занятия с персоналом ЦДС/ДДС филиалов (с использованием методических материалов, размещённых на ВКД_ОДС_СЦУКС) проведены в июне 2025. Основание: «План-график проведения теоретических и практических занятий с дежурными диспетчерами ЦДС филиалов по оперативному реагированию на ЧС (угрозу), происшествие в 2025 году», утвержденный на заседании КЧС и ПБ Общества (п. 9 протокола заседания КЧС и ПБ Общества от 04.03.2025 № 25-ЦА-00110-ПР).п.п. 3, 4, 5, 6, 7 – приняты к исполнению (выполняются при наличии оперативных событий 1, 2 уровня, ЧС (угрозы)). п. 9 – принят к исполнению (выполняется по результатам тренировки, проводимой СЦУКС ПАО «НК «Роснефть» с персоналом ДДС/работниками, ответственными за получение и передачу оперативной информации и работниками, уполномоченными на решение задач в области ГОЧС по вопросам реагирования при возникновении оперативных событий). Тренировок в 2025 году не проводилось.п.п. 10,11 – не применимы (выполняются только в отношении указанных в протоколе ОГ).ответа не требует##16.07.2025</t>
+    <t>п. 2 – проведено совещание с работниками Блока ПБОТОС и ГОЧС (Протокол ВКС от 11.07.2025 №26). В целях уточнения п. 9.7.1 Методических указаний Компании «Взаимодействие с подрядными организациями в области промышленной и пожарной безопасности, охраны труда и окружающей среды» № П3-05 Р-0881 разработан шаблон варианта «Порядка передачи оперативной информации о возникновении (угрозе возникновения) ЧС природного и техногенного характера, происшествия в филиал при оказании услуг и выполнении работ в интересах ООО ИК «СИБИНТЕК»». В филиалах организовано уточнение разработанного шаблона с учетом рода деятельности/вида оказываемых услуг и направление информационных писем в подрядные организации с уточненным порядком передачи оперативной информации при возникновении (угрозе возникновения) ЧС природного и техногенного характера, происшествия во время оказания услуги и/или выполнения работы по договорам с ООО ИК «СИБИНТЕК» на объектах Компании или Общества.п.8 – учебные занятия с персоналом ЦДС/ДДС филиалов (с использованием методических материалов, размещённых на ВКД_ОДС_СЦУКС) проведены в июне 2025. Основание: «План-график проведения теоретических и практических занятий с дежурными диспетчерами ЦДС филиалов по оперативному реагированию на ЧС (угрозу), происшествие в 2025 году», утвержденный на заседании КЧС и ПБ Общества (п. 9 протокола заседания КЧС и ПБ Общества от 04.03.2025 № 25-ЦА-00110-ПР).п.п. 3, 4, 5, 6, 7 – приняты к исполнению (выполняются при наличии оперативных событий 1, 2 уровня, ЧС (угрозы)). п. 9 – принят к исполнению (выполняется по результатам тренировки, проводимой СЦУКС ПАО «НК «Роснефть» с персоналом ДДС/работниками, ответственными за получение и передачу оперативной информации и работниками, уполномоченными на решение задач в области ГОЧС по вопросам реагирования при возникновении оперативных событий). Тренировок в 2025 году не проводилось.п.п. 10,11 – не применимы (выполняются только в отношении указанных в протоколе ОГ).ответа не требует 16.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/4c809163-760d-4461-8b9a-dc76dbd3ae4b</t>
@@ -910,16 +910,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/2de5fb03-41bd-4426-aac3-0a6be1950966</t>
   </si>
   <si>
-    <t>0551-02311-25##03.07.2025</t>
+    <t>0551-02311-25 03.07.2025</t>
   </si>
   <si>
     <t>О запросе обновленного ТКП</t>
   </si>
   <si>
-    <t>ИП-00161-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Принято к сведению. Исп. Загидуллин И.В.##16.07.2025</t>
+    <t>ИП-00161-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Принято к сведению. Исп. Загидуллин И.В. 16.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/69b3f68e-f704-42a8-a097-2167551d3bd7</t>
@@ -928,16 +928,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/7f4f681f-bdcd-42da-a9f0-66d025708135</t>
   </si>
   <si>
-    <t>0551-02309-25##03.07.2025</t>
+    <t>0551-02309-25 03.07.2025</t>
   </si>
   <si>
     <t>О мерах по повышению защищенности информационной инфраструктуры Российской Федерации</t>
   </si>
   <si>
-    <t>ИП-00162-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Ответ направлен от 25.07.2025 № ИСХ-ЦА-02134-25##25.07.2025</t>
+    <t>ИП-00162-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Ответ направлен от 25.07.2025 № ИСХ-ЦА-02134-25 25.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/3b8b9af2-d57c-4b71-9292-68e47a94c45c</t>
@@ -946,16 +946,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/0a445fb4-8138-4170-bff7-52b031ce2bed</t>
   </si>
   <si>
-    <t>0551-02306-25##03.07.2025</t>
+    <t>0551-02306-25 03.07.2025</t>
   </si>
   <si>
     <t>Определение о принятии заявления в порядке упрощенного производства_ООО "ATM АЛЬЯНС СОЛЮШИНС"</t>
   </si>
   <si>
-    <t>ИП-00165-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Передано в  работу представителю по делу для подготовки отзыва на заявление о взыскании судебных расходов.##04.07.2025</t>
+    <t>ИП-00165-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Передано в  работу представителю по делу для подготовки отзыва на заявление о взыскании судебных расходов. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/d6c2cc04-26b0-44eb-8e72-59da2ba3dabb</t>
@@ -964,19 +964,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/a224bec5-3423-4d38-9f86-041e4e6aa7c1</t>
   </si>
   <si>
-    <t>0551-02303-25##03.07.2025</t>
+    <t>0551-02303-25 03.07.2025</t>
   </si>
   <si>
     <t>Об организации встречи</t>
   </si>
   <si>
-    <t>ИП-00166-АИ-25##03.07.2025</t>
+    <t>ИП-00166-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>Для рассмотрения возможности сотрудничества</t>
   </si>
   <si>
-    <t>Учтено в работе, доведено до ЦК импортозамещения в области ПАМиКК (руководитель ЦК - Сорокин Е.Е,). Работа по включению поставщика в Реестр компаний поставщиков/производителей организована.##04.07.2025</t>
+    <t>Учтено в работе, доведено до ЦК импортозамещения в области ПАМиКК (руководитель ЦК - Сорокин Е.Е,). Работа по включению поставщика в Реестр компаний поставщиков/производителей организована. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/0a9581b2-755a-4743-98ce-043776eac788</t>
@@ -985,13 +985,13 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/b1f61dcc-cf9a-4fa1-b75c-556d04a1136f</t>
   </si>
   <si>
-    <t>0551-02270-25##03.07.2025</t>
+    <t>0551-02270-25 03.07.2025</t>
   </si>
   <si>
     <t>О подготовке материалов для защитыбизнес-плана на 2026-2030 годы</t>
   </si>
   <si>
-    <t>ИП-00167-АИ-25##03.07.2025</t>
+    <t>ИП-00167-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>15.08.2025</t>
@@ -1000,7 +1000,7 @@
     <t>14.08.2025</t>
   </si>
   <si>
-    <t>Информация направлена на указанные в запросе ИСХ-19-17777-25 адреса эл. почты.Факт отправки во вложении.##14.08.2025</t>
+    <t>Информация направлена на указанные в запросе ИСХ-19-17777-25 адреса эл. почты.Факт отправки во вложении. 14.08.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/34c8db58-1967-42d1-9e3f-89616a8ebdab</t>
@@ -1009,19 +1009,19 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/1fc62885-5d00-403f-a688-06c88e8b1d8e</t>
   </si>
   <si>
-    <t>0551-02268-25##03.07.2025</t>
+    <t>0551-02268-25 03.07.2025</t>
   </si>
   <si>
     <t>О форме сбора данных Раздел 20 "Собственность и корпоративное управление"</t>
   </si>
   <si>
-    <t>ИП-00168-АИ-25##03.07.2025</t>
+    <t>ИП-00168-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>В части направления первоначальной версии</t>
   </si>
   <si>
-    <t>Р-20 ООО ИК Сибинтек верс "сентябрь" загружена на согласование в SAP 01.08.25##01.08.2025</t>
+    <t>Р-20 ООО ИК Сибинтек верс "сентябрь" загружена на согласование в SAP 01.08.25 01.08.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/562390b2-2868-4120-b139-0ff044edfd23</t>
@@ -1030,7 +1030,7 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/44bac6e0-5ab5-458c-ab28-18a06e46b755</t>
   </si>
   <si>
-    <t>ИП-00169-АИ-25##03.07.2025</t>
+    <t>ИП-00169-АИ-25 03.07.2025</t>
   </si>
   <si>
     <t>В части направления окончательной версии</t>
@@ -1042,16 +1042,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/bf266cd7-899f-4aaf-88bb-236a328ec991</t>
   </si>
   <si>
-    <t>0551-02251-25##03.07.2025</t>
+    <t>0551-02251-25 03.07.2025</t>
   </si>
   <si>
     <t>О предоставлении информации об освоенных объемах инвестиций в Салаватском районе</t>
   </si>
   <si>
-    <t>ИП-00170-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Направлено письмо  №ИСХ-МБ-00748-25 от 09.07.2025##11.07.2025</t>
+    <t>ИП-00170-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Направлено письмо  №ИСХ-МБ-00748-25 от 09.07.2025 11.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/1bcb9cf0-0d18-4f6a-a1b2-226d86b0b46b</t>
@@ -1060,16 +1060,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/6bbe9d5f-ada8-4c08-a68c-d0847451f730</t>
   </si>
   <si>
-    <t>0551-02246-25##03.07.2025</t>
+    <t>0551-02246-25 03.07.2025</t>
   </si>
   <si>
     <t>О перераспределении запасов для нужд ООО ЧОП "РН-Охрана-Краснодар"</t>
   </si>
   <si>
-    <t>ИП-00171-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Ответ в рабочем порядке направлен на почту chop@krasnodar.rn-ohrana.ru (Перечень СВЗ/НВЛ запасов для самостоятельного анализа).##09.07.2025</t>
+    <t>ИП-00171-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Ответ в рабочем порядке направлен на почту chop@krasnodar.rn-ohrana.ru (Перечень СВЗ/НВЛ запасов для самостоятельного анализа). 09.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/8503ac6a-d71a-4a6d-94c2-235ec23764e0</t>
@@ -1078,16 +1078,16 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/f5af68db-1efb-442c-b452-a88ce55fb365</t>
   </si>
   <si>
-    <t>0551-02225-25##03.07.2025</t>
+    <t>0551-02225-25 03.07.2025</t>
   </si>
   <si>
     <t>Определение о принятии кассационной жалобы к производству суда_Бойчук А.Н.</t>
   </si>
   <si>
-    <t>ИП-00172-АИ-25##03.07.2025</t>
-  </si>
-  <si>
-    <t>Передано в работу судебному представителю для подготовки отзыва на жалобу.##04.07.2025</t>
+    <t>ИП-00172-АИ-25 03.07.2025</t>
+  </si>
+  <si>
+    <t>Передано в работу судебному представителю для подготовки отзыва на жалобу. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/98dfd853-5f93-4b01-989b-3bad7902df3d</t>
@@ -1096,7 +1096,7 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/42f92175-9756-4d13-b7bb-73581ad93f7e</t>
   </si>
   <si>
-    <t>ИП-00707-ЦА-25##17.07.2025</t>
+    <t>ИП-00707-ЦА-25 17.07.2025</t>
   </si>
   <si>
     <t>Исполнить документ (оригинал необходимо забрать в приемной ГД)</t>
@@ -1108,7 +1108,7 @@
     <t>На проверке отчета</t>
   </si>
   <si>
-    <t>Принято.##15.08.2025</t>
+    <t>Принято. 15.08.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/8d42034f-0113-492c-ae06-a091ebc25a4a</t>
@@ -1117,7 +1117,7 @@
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/9c83cdff-0ac6-4c54-8a2a-a05d29978401</t>
   </si>
   <si>
-    <t>Принято для учета и оценки результатов деятельности проектной команды.##04.07.2025</t>
+    <t>Принято для учета и оценки результатов деятельности проектной команды. 04.07.2025</t>
   </si>
   <si>
     <t>https://og-5.ksed.rosneft.ru/share/page/document?nodeRef=workspace://SpacesStore/9c10abc5-9bdd-4079-bea6-9faf3f5106e5</t>

</xml_diff>